<commit_message>
Styling Updates - finishing touches
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="156">
   <si>
     <t>Browser</t>
   </si>
@@ -1518,9 +1518,6 @@
   </si>
   <si>
     <t>o   STRETCH – change results to not use e-mails as identifiers.</t>
-  </si>
-  <si>
-    <t>Figure out if no group yet…</t>
   </si>
   <si>
     <t>Prefs page?</t>
@@ -2153,9 +2150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2197,11 +2194,8 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
+      <c r="A5" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2211,27 +2205,11 @@
       <c r="A7" s="5"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="5" t="s">
+      <c r="A8" s="7"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="18" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="18" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1"/>
@@ -2611,7 +2589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
@@ -3140,7 +3118,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:2">

</xml_diff>